<commit_message>
Adding ClickHandler that clicks on element at specified path
</commit_message>
<xml_diff>
--- a/src/main/resources/input.xlsx
+++ b/src/main/resources/input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="561" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" tabRatio="561" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Y</t>
   </si>
@@ -101,13 +101,19 @@
   </si>
   <si>
     <t>testCase</t>
+  </si>
+  <si>
+    <t>Check Today's Deals</t>
+  </si>
+  <si>
+    <t>.//*[@id='nav-xshop']/a[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,6 +145,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -185,7 +197,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,6 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -558,7 +571,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,13 +585,13 @@
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="48.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="48.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -586,42 +599,42 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -642,26 +655,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:I5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="26.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="31.81640625" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" customWidth="1"/>
+    <col min="8" max="8" width="26.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -691,7 +704,7 @@
       </c>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -717,71 +730,93 @@
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Adding CheckCurrentUrlHandler that gets and verifies the current url the browser is pointing to
</commit_message>
<xml_diff>
--- a/src/main/resources/input.xlsx
+++ b/src/main/resources/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Y</t>
   </si>
@@ -55,9 +55,6 @@
     <t>IS_DISPLAYED</t>
   </si>
   <si>
-    <t>GET_CURRENT_URL</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -107,6 +104,18 @@
   </si>
   <si>
     <t>.//*[@id='nav-xshop']/a[2]</t>
+  </si>
+  <si>
+    <t>CHECK_CURRENT_URL</t>
+  </si>
+  <si>
+    <t>Verify url in address bar</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>ref=nav_topnav_deals</t>
   </si>
 </sst>
 </file>
@@ -582,7 +591,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,7 +605,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -611,7 +620,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -636,7 +645,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -655,10 +664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,31 +685,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="J1" s="4"/>
     </row>
@@ -712,19 +721,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="3"/>
@@ -738,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
@@ -748,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -759,44 +768,51 @@
       <c r="D4" s="5">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -806,10 +822,25 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adding 'IS_CLICKABLE' handler that checks if an item on the page is clickable
</commit_message>
<xml_diff>
--- a/src/main/resources/input.xlsx
+++ b/src/main/resources/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Y</t>
   </si>
@@ -34,9 +34,6 @@
     <t>xpath</t>
   </si>
   <si>
-    <t>html/body/div[1]/div/div/div[2]/a/span</t>
-  </si>
-  <si>
     <t>NAVIGATE_TO</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>ref=nav_topnav_deals</t>
+  </si>
+  <si>
+    <t>Check if Today's Deals link is clickable</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,6 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="18" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -605,47 +606,47 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -664,10 +665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,31 +686,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="J1" s="4"/>
     </row>
@@ -721,19 +722,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="3"/>
@@ -747,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
@@ -757,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -769,17 +770,17 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="5" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -790,44 +791,51 @@
       <c r="D5" s="5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="3"/>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -837,10 +845,21 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>